<commit_message>
visualization + working 30 iteration cross validation
</commit_message>
<xml_diff>
--- a/notebooks/output/accs.xlsx
+++ b/notebooks/output/accs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itznu\PycharmProjects\use-of-snn\notebooks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D86D1DB-8BAC-4C7F-AAD6-352491E6FF95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F95A50-36C8-43AE-A1C8-EFF4F939B023}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -50,6 +50,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,11 +103,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +424,7 @@
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,7 +435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -439,8 +445,16 @@
       <c r="C2">
         <v>6.9116743671528286E-3</v>
       </c>
+      <c r="E2" s="2">
+        <f>B2*100</f>
+        <v>64.073333144187927</v>
+      </c>
+      <c r="F2" s="3">
+        <f>C2</f>
+        <v>6.9116743671528286E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -450,8 +464,16 @@
       <c r="C3">
         <v>6.713050995913644E-3</v>
       </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E6" si="0">B3*100</f>
+        <v>64.106520657043305</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F6" si="1">C3</f>
+        <v>6.713050995913644E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -461,8 +483,16 @@
       <c r="C4">
         <v>1.2482515936564119E-2</v>
       </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>53.281898125103702</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.2482515936564119E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -472,8 +502,16 @@
       <c r="C5">
         <v>6.9976779250982366E-3</v>
       </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>64.104861456777826</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>6.9976779250982366E-3</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -481,10 +519,19 @@
         <v>0.52877053260328521</v>
       </c>
       <c r="C6">
+        <v>1.335448131153358E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>52.877053260328523</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
         <v>1.335448131153358E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>